<commit_message>
added 2 more new offers
</commit_message>
<xml_diff>
--- a/Updates/Input data/8682-AdvancedActionListi.xlsx
+++ b/Updates/Input data/8682-AdvancedActionListi.xlsx
@@ -123,7 +123,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -178,11 +178,11 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>45955.97105324074</v>
+        <v>45957.87008101852</v>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6507.659333</t>
+          <t>M.15608.6509.483847</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -201,14 +201,14 @@
         </is>
       </c>
       <c r="F2" s="6" t="n">
-        <v>44.72</v>
+        <v>78.92</v>
       </c>
       <c r="G2" s="7" t="n">
-        <v>4.47</v>
+        <v>7.89</v>
       </c>
       <c r="H2" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I2" s="9" t="inlineStr">
@@ -219,11 +219,11 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>45955.847719907404</v>
+        <v>45957.73342592592</v>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6507.395050</t>
+          <t>M.15608.6509.183321</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
@@ -242,10 +242,10 @@
         </is>
       </c>
       <c r="F3" s="6" t="n">
-        <v>87.94</v>
+        <v>104.35</v>
       </c>
       <c r="G3" s="7" t="n">
-        <v>8.79</v>
+        <v>10.44</v>
       </c>
       <c r="H3" s="8" t="inlineStr">
         <is>
@@ -260,11 +260,11 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>45955.39493055556</v>
+        <v>45957.62462962963</v>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6506.1443638</t>
+          <t>M.15608.6509.65463</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -283,14 +283,14 @@
         </is>
       </c>
       <c r="F4" s="6" t="n">
-        <v>87.94</v>
+        <v>34.73</v>
       </c>
       <c r="G4" s="7" t="n">
-        <v>8.79</v>
+        <v>3.47</v>
       </c>
       <c r="H4" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I4" s="9" t="inlineStr">
@@ -301,11 +301,11 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>45954.92899305555</v>
+        <v>45957.601851851854</v>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6506.583818</t>
+          <t>M.15608.6509.49402</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
@@ -324,14 +324,14 @@
         </is>
       </c>
       <c r="F5" s="6" t="n">
-        <v>81.96</v>
+        <v>14.21</v>
       </c>
       <c r="G5" s="7" t="n">
-        <v>8.2</v>
+        <v>1.42</v>
       </c>
       <c r="H5" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I5" s="9" t="inlineStr">
@@ -342,11 +342,11 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>45954.87305555555</v>
+        <v>45957.60162037037</v>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6506.459388</t>
+          <t>M.15608.6509.49340</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
@@ -365,10 +365,10 @@
         </is>
       </c>
       <c r="F6" s="6" t="n">
-        <v>52.15</v>
+        <v>61.1</v>
       </c>
       <c r="G6" s="7" t="n">
-        <v>5.22</v>
+        <v>6.11</v>
       </c>
       <c r="H6" s="8" t="inlineStr">
         <is>
@@ -383,11 +383,11 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>45954.84951388889</v>
+        <v>45957.492939814816</v>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6506.405561</t>
+          <t>M.15608.6508.1758842</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
@@ -406,14 +406,14 @@
         </is>
       </c>
       <c r="F7" s="6" t="n">
-        <v>110.48</v>
+        <v>104.35</v>
       </c>
       <c r="G7" s="7" t="n">
-        <v>11.05</v>
+        <v>10.44</v>
       </c>
       <c r="H7" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I7" s="9" t="inlineStr">
@@ -424,11 +424,11 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>45954.71026620371</v>
+        <v>45957.21574074074</v>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6506.159942</t>
+          <t>M.15608.6508.1354778</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
@@ -447,10 +447,10 @@
         </is>
       </c>
       <c r="F8" s="6" t="n">
-        <v>14.2</v>
+        <v>115.23</v>
       </c>
       <c r="G8" s="7" t="n">
-        <v>1.42</v>
+        <v>11.52</v>
       </c>
       <c r="H8" s="8" t="inlineStr">
         <is>
@@ -465,11 +465,11 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>45954.67798611111</v>
+        <v>45957.147824074076</v>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6506.113392</t>
+          <t>M.15608.6508.1186647</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
@@ -488,10 +488,10 @@
         </is>
       </c>
       <c r="F9" s="6" t="n">
-        <v>14.2</v>
+        <v>75.77</v>
       </c>
       <c r="G9" s="7" t="n">
-        <v>1.42</v>
+        <v>7.58</v>
       </c>
       <c r="H9" s="8" t="inlineStr">
         <is>
@@ -506,11 +506,11 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>45954.631006944444</v>
+        <v>45957.14303240741</v>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6506.72786</t>
+          <t>M.15608.6508.1176092</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
@@ -529,14 +529,14 @@
         </is>
       </c>
       <c r="F10" s="6" t="n">
-        <v>36.3</v>
+        <v>43.22</v>
       </c>
       <c r="G10" s="7" t="n">
-        <v>3.63</v>
+        <v>4.32</v>
       </c>
       <c r="H10" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I10" s="9" t="inlineStr">
@@ -547,11 +547,11 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>45954.560625</v>
+        <v>45957.00587962963</v>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6506.31202</t>
+          <t>M.15608.6508.806263</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
@@ -570,10 +570,10 @@
         </is>
       </c>
       <c r="F11" s="6" t="n">
-        <v>93.12</v>
+        <v>47.35</v>
       </c>
       <c r="G11" s="7" t="n">
-        <v>9.31</v>
+        <v>4.74</v>
       </c>
       <c r="H11" s="8" t="inlineStr">
         <is>
@@ -588,11 +588,11 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>45954.52207175926</v>
+        <v>45956.7049537037</v>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6506.12675</t>
+          <t>M.15608.6508.144728</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
@@ -611,10 +611,10 @@
         </is>
       </c>
       <c r="F12" s="6" t="n">
-        <v>110.48</v>
+        <v>36.3</v>
       </c>
       <c r="G12" s="7" t="n">
-        <v>11.05</v>
+        <v>3.63</v>
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
@@ -629,11 +629,11 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>45954.42665509259</v>
+        <v>45956.61803240741</v>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6505.1304413</t>
+          <t>M.15608.6508.57430</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
@@ -652,14 +652,14 @@
         </is>
       </c>
       <c r="F13" s="6" t="n">
-        <v>58.4</v>
+        <v>56.65</v>
       </c>
       <c r="G13" s="7" t="n">
-        <v>5.84</v>
+        <v>5.66</v>
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I13" s="9" t="inlineStr">
@@ -670,11 +670,11 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>45954.397141203706</v>
+        <v>45956.60287037037</v>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6505.1271862</t>
+          <t>M.15608.6508.48507</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
@@ -693,14 +693,14 @@
         </is>
       </c>
       <c r="F14" s="6" t="n">
-        <v>104.34</v>
+        <v>37.88</v>
       </c>
       <c r="G14" s="7" t="n">
-        <v>10.43</v>
+        <v>3.79</v>
       </c>
       <c r="H14" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I14" s="9" t="inlineStr">
@@ -711,11 +711,11 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>45954.37380787037</v>
+        <v>45956.60021990741</v>
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6505.1255452</t>
+          <t>M.15608.6508.46696</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
@@ -734,14 +734,14 @@
         </is>
       </c>
       <c r="F15" s="6" t="n">
-        <v>26.83</v>
+        <v>14.21</v>
       </c>
       <c r="G15" s="7" t="n">
-        <v>2.68</v>
+        <v>1.42</v>
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I15" s="9" t="inlineStr">
@@ -752,11 +752,11 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>45954.24269675926</v>
+        <v>45956.541666666664</v>
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6505.1102880</t>
+          <t>M.15608.6508.20795</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
@@ -775,14 +775,14 @@
         </is>
       </c>
       <c r="F16" s="6" t="n">
-        <v>118.37</v>
+        <v>13.4</v>
       </c>
       <c r="G16" s="7" t="n">
-        <v>11.84</v>
+        <v>1.34</v>
       </c>
       <c r="H16" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I16" s="9" t="inlineStr">
@@ -793,11 +793,11 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>45954.16863425926</v>
+        <v>45956.42675925926</v>
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6505.1005197</t>
+          <t>M.15608.6507.1577125</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
@@ -816,14 +816,14 @@
         </is>
       </c>
       <c r="F17" s="6" t="n">
-        <v>52.15</v>
+        <v>59.98</v>
       </c>
       <c r="G17" s="7" t="n">
-        <v>5.22</v>
+        <v>6.0</v>
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I17" s="9" t="inlineStr">
@@ -834,11 +834,11 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>45954.07134259259</v>
+        <v>45956.22388888889</v>
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6505.791230</t>
+          <t>M.15608.6507.1258171</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
@@ -857,14 +857,14 @@
         </is>
       </c>
       <c r="F18" s="6" t="n">
-        <v>81.96</v>
+        <v>15.78</v>
       </c>
       <c r="G18" s="7" t="n">
-        <v>8.2</v>
+        <v>1.58</v>
       </c>
       <c r="H18" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I18" s="9" t="inlineStr">
@@ -875,11 +875,11 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>45954.00981481482</v>
+        <v>45956.009930555556</v>
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6505.721227</t>
+          <t>M.15608.6507.741958</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
@@ -898,10 +898,10 @@
         </is>
       </c>
       <c r="F19" s="6" t="n">
-        <v>14.2</v>
+        <v>39.46</v>
       </c>
       <c r="G19" s="7" t="n">
-        <v>1.42</v>
+        <v>3.95</v>
       </c>
       <c r="H19" s="8" t="inlineStr">
         <is>
@@ -916,11 +916,11 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>45953.87228009259</v>
+        <v>45955.97105324074</v>
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6505.491801</t>
+          <t>M.15608.6507.659333</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
@@ -939,14 +939,14 @@
         </is>
       </c>
       <c r="F20" s="6" t="n">
-        <v>77.33</v>
+        <v>44.72</v>
       </c>
       <c r="G20" s="7" t="n">
-        <v>7.73</v>
+        <v>4.47</v>
       </c>
       <c r="H20" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I20" s="9" t="inlineStr">
@@ -957,11 +957,11 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>45953.85863425926</v>
+        <v>45955.847719907404</v>
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6505.430950</t>
+          <t>M.15608.6507.395050</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
@@ -980,10 +980,10 @@
         </is>
       </c>
       <c r="F21" s="6" t="n">
-        <v>56.64</v>
+        <v>87.94</v>
       </c>
       <c r="G21" s="7" t="n">
-        <v>5.66</v>
+        <v>8.79</v>
       </c>
       <c r="H21" s="8" t="inlineStr">
         <is>
@@ -998,11 +998,11 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>45953.83896990741</v>
+        <v>45955.39493055556</v>
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6505.403682</t>
+          <t>M.15608.6506.1443638</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
@@ -1021,14 +1021,14 @@
         </is>
       </c>
       <c r="F22" s="6" t="n">
-        <v>14.2</v>
+        <v>87.94</v>
       </c>
       <c r="G22" s="7" t="n">
-        <v>1.42</v>
+        <v>8.79</v>
       </c>
       <c r="H22" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I22" s="9" t="inlineStr">
@@ -1039,11 +1039,11 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>45953.73425925926</v>
+        <v>45954.92899305555</v>
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6505.201014</t>
+          <t>M.15608.6506.583818</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
@@ -1062,14 +1062,14 @@
         </is>
       </c>
       <c r="F23" s="6" t="n">
-        <v>71.02</v>
+        <v>81.96</v>
       </c>
       <c r="G23" s="7" t="n">
-        <v>7.1</v>
+        <v>8.2</v>
       </c>
       <c r="H23" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I23" s="9" t="inlineStr">
@@ -1080,11 +1080,11 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>45953.630474537036</v>
+        <v>45954.87305555555</v>
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6505.65255</t>
+          <t>M.15608.6506.459388</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
@@ -1103,14 +1103,14 @@
         </is>
       </c>
       <c r="F24" s="6" t="n">
-        <v>36.3</v>
+        <v>52.15</v>
       </c>
       <c r="G24" s="7" t="n">
-        <v>3.63</v>
+        <v>5.22</v>
       </c>
       <c r="H24" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I24" s="9" t="inlineStr">
@@ -1121,11 +1121,11 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>45953.62299768518</v>
+        <v>45954.84951388889</v>
       </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6505.59928</t>
+          <t>M.15608.6506.405561</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
@@ -1144,10 +1144,10 @@
         </is>
       </c>
       <c r="F25" s="6" t="n">
-        <v>71.02</v>
+        <v>110.48</v>
       </c>
       <c r="G25" s="7" t="n">
-        <v>7.1</v>
+        <v>11.05</v>
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
@@ -1162,11 +1162,11 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>45953.59605324074</v>
+        <v>45954.71026620371</v>
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6505.44409</t>
+          <t>M.15608.6506.159942</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
@@ -1185,10 +1185,10 @@
         </is>
       </c>
       <c r="F26" s="6" t="n">
-        <v>59.97</v>
+        <v>14.2</v>
       </c>
       <c r="G26" s="7" t="n">
-        <v>6.0</v>
+        <v>1.42</v>
       </c>
       <c r="H26" s="8" t="inlineStr">
         <is>
@@ -1203,11 +1203,11 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>45953.35972222222</v>
+        <v>45954.67798611111</v>
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6504.1306645</t>
+          <t>M.15608.6506.113392</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
@@ -1226,10 +1226,10 @@
         </is>
       </c>
       <c r="F27" s="6" t="n">
-        <v>42.61</v>
+        <v>14.2</v>
       </c>
       <c r="G27" s="7" t="n">
-        <v>4.26</v>
+        <v>1.42</v>
       </c>
       <c r="H27" s="8" t="inlineStr">
         <is>
@@ -1244,11 +1244,11 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>45953.086851851855</v>
+        <v>45954.631006944444</v>
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6504.855829</t>
+          <t>M.15608.6506.72786</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
@@ -1267,10 +1267,10 @@
         </is>
       </c>
       <c r="F28" s="6" t="n">
-        <v>61.55</v>
+        <v>36.3</v>
       </c>
       <c r="G28" s="7" t="n">
-        <v>6.16</v>
+        <v>3.63</v>
       </c>
       <c r="H28" s="8" t="inlineStr">
         <is>
@@ -1285,11 +1285,11 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>45953.019780092596</v>
+        <v>45954.560625</v>
       </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6504.753206</t>
+          <t>M.15608.6506.31202</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
@@ -1308,14 +1308,14 @@
         </is>
       </c>
       <c r="F29" s="6" t="n">
-        <v>29.3</v>
+        <v>93.12</v>
       </c>
       <c r="G29" s="7" t="n">
-        <v>2.93</v>
+        <v>9.31</v>
       </c>
       <c r="H29" s="8" t="inlineStr">
         <is>
-          <t>D20</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I29" s="9" t="inlineStr">
@@ -1326,11 +1326,11 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>45952.97883101852</v>
+        <v>45954.52207175926</v>
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6504.694549</t>
+          <t>M.15608.6506.12675</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
@@ -1349,10 +1349,10 @@
         </is>
       </c>
       <c r="F30" s="6" t="n">
-        <v>26.83</v>
+        <v>110.48</v>
       </c>
       <c r="G30" s="7" t="n">
-        <v>2.68</v>
+        <v>11.05</v>
       </c>
       <c r="H30" s="8" t="inlineStr">
         <is>
@@ -1367,11 +1367,11 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>45952.963692129626</v>
+        <v>45954.42665509259</v>
       </c>
       <c r="B31" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6504.672763</t>
+          <t>M.15608.6505.1304413</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
@@ -1390,14 +1390,14 @@
         </is>
       </c>
       <c r="F31" s="6" t="n">
-        <v>45.78</v>
+        <v>58.4</v>
       </c>
       <c r="G31" s="7" t="n">
-        <v>4.58</v>
+        <v>5.84</v>
       </c>
       <c r="H31" s="8" t="inlineStr">
         <is>
-          <t>D26</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I31" s="9" t="inlineStr">
@@ -1408,11 +1408,11 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>45952.761770833335</v>
+        <v>45954.397141203706</v>
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6504.259796</t>
+          <t>M.15608.6505.1271862</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
@@ -1431,14 +1431,14 @@
         </is>
       </c>
       <c r="F32" s="6" t="n">
-        <v>14.21</v>
+        <v>104.34</v>
       </c>
       <c r="G32" s="7" t="n">
-        <v>1.42</v>
+        <v>10.43</v>
       </c>
       <c r="H32" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I32" s="9" t="inlineStr">
@@ -1449,11 +1449,11 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>45952.73630787037</v>
+        <v>45954.37380787037</v>
       </c>
       <c r="B33" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6504.209654</t>
+          <t>M.15608.6505.1255452</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
@@ -1472,14 +1472,14 @@
         </is>
       </c>
       <c r="F33" s="6" t="n">
-        <v>124.7</v>
+        <v>26.83</v>
       </c>
       <c r="G33" s="7" t="n">
-        <v>12.47</v>
+        <v>2.68</v>
       </c>
       <c r="H33" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I33" s="9" t="inlineStr">
@@ -1490,11 +1490,11 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>45952.685532407406</v>
+        <v>45954.24269675926</v>
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6504.125010</t>
+          <t>M.15608.6505.1102880</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
@@ -1513,10 +1513,10 @@
         </is>
       </c>
       <c r="F34" s="6" t="n">
-        <v>37.88</v>
+        <v>118.37</v>
       </c>
       <c r="G34" s="7" t="n">
-        <v>3.79</v>
+        <v>11.84</v>
       </c>
       <c r="H34" s="8" t="inlineStr">
         <is>
@@ -1531,11 +1531,11 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>45952.66378472222</v>
+        <v>45954.16863425926</v>
       </c>
       <c r="B35" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6504.107621</t>
+          <t>M.15608.6505.1005197</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
@@ -1554,14 +1554,14 @@
         </is>
       </c>
       <c r="F35" s="6" t="n">
-        <v>39.46</v>
+        <v>52.15</v>
       </c>
       <c r="G35" s="7" t="n">
-        <v>3.95</v>
+        <v>5.22</v>
       </c>
       <c r="H35" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I35" s="9" t="inlineStr">
@@ -1572,11 +1572,11 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>45952.63895833334</v>
+        <v>45954.07134259259</v>
       </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6504.78271</t>
+          <t>M.15608.6505.791230</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
@@ -1595,14 +1595,14 @@
         </is>
       </c>
       <c r="F36" s="6" t="n">
-        <v>34.73</v>
+        <v>81.96</v>
       </c>
       <c r="G36" s="7" t="n">
-        <v>3.47</v>
+        <v>8.2</v>
       </c>
       <c r="H36" s="8" t="inlineStr">
         <is>
-          <t>D26</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I36" s="9" t="inlineStr">
@@ -1613,11 +1613,11 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>45952.633784722224</v>
+        <v>45954.00981481482</v>
       </c>
       <c r="B37" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6504.73385</t>
+          <t>M.15608.6505.721227</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
@@ -1636,14 +1636,14 @@
         </is>
       </c>
       <c r="F37" s="6" t="n">
-        <v>14.21</v>
+        <v>14.2</v>
       </c>
       <c r="G37" s="7" t="n">
         <v>1.42</v>
       </c>
       <c r="H37" s="8" t="inlineStr">
         <is>
-          <t>D33</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I37" s="9" t="inlineStr">
@@ -1654,11 +1654,11 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>45952.586226851854</v>
+        <v>45953.87228009259</v>
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6504.45896</t>
+          <t>M.15608.6505.491801</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
@@ -1677,14 +1677,14 @@
         </is>
       </c>
       <c r="F38" s="6" t="n">
-        <v>13.4</v>
+        <v>77.33</v>
       </c>
       <c r="G38" s="7" t="n">
-        <v>1.34</v>
+        <v>7.73</v>
       </c>
       <c r="H38" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I38" s="9" t="inlineStr">
@@ -1695,11 +1695,11 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>45952.560069444444</v>
+        <v>45953.85863425926</v>
       </c>
       <c r="B39" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6504.34027</t>
+          <t>M.15608.6505.430950</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
@@ -1718,14 +1718,14 @@
         </is>
       </c>
       <c r="F39" s="6" t="n">
-        <v>36.3</v>
+        <v>56.64</v>
       </c>
       <c r="G39" s="7" t="n">
-        <v>3.63</v>
+        <v>5.66</v>
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I39" s="9" t="inlineStr">
@@ -1736,11 +1736,11 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>45952.487858796296</v>
+        <v>45953.83896990741</v>
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6503.1430691</t>
+          <t>M.15608.6505.403682</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
@@ -1759,14 +1759,14 @@
         </is>
       </c>
       <c r="F40" s="6" t="n">
-        <v>104.35</v>
+        <v>14.2</v>
       </c>
       <c r="G40" s="7" t="n">
-        <v>10.44</v>
+        <v>1.42</v>
       </c>
       <c r="H40" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I40" s="9" t="inlineStr">
@@ -1777,11 +1777,11 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>45952.43483796297</v>
+        <v>45953.73425925926</v>
       </c>
       <c r="B41" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6503.1354508</t>
+          <t>M.15608.6505.201014</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
@@ -1800,10 +1800,10 @@
         </is>
       </c>
       <c r="F41" s="6" t="n">
-        <v>44.2</v>
+        <v>71.02</v>
       </c>
       <c r="G41" s="7" t="n">
-        <v>4.42</v>
+        <v>7.1</v>
       </c>
       <c r="H41" s="8" t="inlineStr">
         <is>
@@ -1818,11 +1818,11 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>45952.12751157407</v>
+        <v>45953.630474537036</v>
       </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6503.747194</t>
+          <t>M.15608.6505.65255</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr">
@@ -1841,10 +1841,10 @@
         </is>
       </c>
       <c r="F42" s="6" t="n">
-        <v>45.78</v>
+        <v>36.3</v>
       </c>
       <c r="G42" s="7" t="n">
-        <v>4.58</v>
+        <v>3.63</v>
       </c>
       <c r="H42" s="8" t="inlineStr">
         <is>
@@ -1859,11 +1859,11 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>45952.00640046296</v>
+        <v>45953.62299768518</v>
       </c>
       <c r="B43" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6503.566392</t>
+          <t>M.15608.6505.59928</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
@@ -1882,14 +1882,14 @@
         </is>
       </c>
       <c r="F43" s="6" t="n">
-        <v>43.22</v>
+        <v>71.02</v>
       </c>
       <c r="G43" s="7" t="n">
-        <v>4.32</v>
+        <v>7.1</v>
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I43" s="9" t="inlineStr">
@@ -1900,11 +1900,11 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>45951.95179398148</v>
+        <v>45953.59605324074</v>
       </c>
       <c r="B44" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6503.460669</t>
+          <t>M.15608.6505.44409</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
@@ -1923,14 +1923,14 @@
         </is>
       </c>
       <c r="F44" s="6" t="n">
-        <v>31.25</v>
+        <v>59.97</v>
       </c>
       <c r="G44" s="7" t="n">
-        <v>3.13</v>
+        <v>6.0</v>
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>D26</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I44" s="9" t="inlineStr">
@@ -1941,11 +1941,11 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>45951.918599537035</v>
+        <v>45953.35972222222</v>
       </c>
       <c r="B45" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6503.413344</t>
+          <t>M.15608.6504.1306645</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
@@ -1964,14 +1964,14 @@
         </is>
       </c>
       <c r="F45" s="6" t="n">
-        <v>26.83</v>
+        <v>42.61</v>
       </c>
       <c r="G45" s="7" t="n">
-        <v>2.68</v>
+        <v>4.26</v>
       </c>
       <c r="H45" s="8" t="inlineStr">
         <is>
-          <t>D26</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I45" s="9" t="inlineStr">
@@ -1982,11 +1982,11 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>45951.695868055554</v>
+        <v>45953.086851851855</v>
       </c>
       <c r="B46" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6503.127414</t>
+          <t>M.15608.6504.855829</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
@@ -2005,10 +2005,10 @@
         </is>
       </c>
       <c r="F46" s="6" t="n">
-        <v>14.21</v>
+        <v>61.55</v>
       </c>
       <c r="G46" s="7" t="n">
-        <v>1.42</v>
+        <v>6.16</v>
       </c>
       <c r="H46" s="8" t="inlineStr">
         <is>
@@ -2023,11 +2023,11 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>45951.63533564815</v>
+        <v>45953.019780092596</v>
       </c>
       <c r="B47" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6503.85823</t>
+          <t>M.15608.6504.753206</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
@@ -2046,14 +2046,14 @@
         </is>
       </c>
       <c r="F47" s="6" t="n">
-        <v>37.25</v>
+        <v>29.3</v>
       </c>
       <c r="G47" s="7" t="n">
-        <v>3.73</v>
+        <v>2.93</v>
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>D20</t>
         </is>
       </c>
       <c r="I47" s="9" t="inlineStr">
@@ -2064,11 +2064,11 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>45951.47851851852</v>
+        <v>45952.97883101852</v>
       </c>
       <c r="B48" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6502.1404826</t>
+          <t>M.15608.6504.694549</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
@@ -2087,14 +2087,14 @@
         </is>
       </c>
       <c r="F48" s="6" t="n">
-        <v>14.21</v>
+        <v>26.83</v>
       </c>
       <c r="G48" s="7" t="n">
-        <v>1.42</v>
+        <v>2.68</v>
       </c>
       <c r="H48" s="8" t="inlineStr">
         <is>
-          <t>D33</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I48" s="9" t="inlineStr">
@@ -2105,11 +2105,11 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>45951.430138888885</v>
+        <v>45952.963692129626</v>
       </c>
       <c r="B49" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6502.1343453</t>
+          <t>M.15608.6504.672763</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
@@ -2128,14 +2128,14 @@
         </is>
       </c>
       <c r="F49" s="6" t="n">
-        <v>36.3</v>
+        <v>45.78</v>
       </c>
       <c r="G49" s="7" t="n">
-        <v>3.63</v>
+        <v>4.58</v>
       </c>
       <c r="H49" s="8" t="inlineStr">
         <is>
-          <t>D7</t>
+          <t>D26</t>
         </is>
       </c>
       <c r="I49" s="9" t="inlineStr">
@@ -2146,11 +2146,11 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>45951.35328703704</v>
+        <v>45952.761770833335</v>
       </c>
       <c r="B50" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6502.1251979</t>
+          <t>M.15608.6504.259796</t>
         </is>
       </c>
       <c r="C50" s="3" t="inlineStr">
@@ -2169,10 +2169,10 @@
         </is>
       </c>
       <c r="F50" s="6" t="n">
-        <v>110.49</v>
+        <v>14.21</v>
       </c>
       <c r="G50" s="7" t="n">
-        <v>11.05</v>
+        <v>1.42</v>
       </c>
       <c r="H50" s="8" t="inlineStr">
         <is>
@@ -2187,11 +2187,11 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>45951.28636574074</v>
+        <v>45952.73630787037</v>
       </c>
       <c r="B51" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6502.1182640</t>
+          <t>M.15608.6504.209654</t>
         </is>
       </c>
       <c r="C51" s="3" t="inlineStr">
@@ -2210,10 +2210,10 @@
         </is>
       </c>
       <c r="F51" s="6" t="n">
-        <v>64.72</v>
+        <v>124.7</v>
       </c>
       <c r="G51" s="7" t="n">
-        <v>6.47</v>
+        <v>12.47</v>
       </c>
       <c r="H51" s="8" t="inlineStr">
         <is>
@@ -2228,11 +2228,11 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>45950.9299537037</v>
+        <v>45952.685532407406</v>
       </c>
       <c r="B52" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6502.517328</t>
+          <t>M.15608.6504.125010</t>
         </is>
       </c>
       <c r="C52" s="3" t="inlineStr">
@@ -2251,14 +2251,14 @@
         </is>
       </c>
       <c r="F52" s="6" t="n">
-        <v>86.8</v>
+        <v>37.88</v>
       </c>
       <c r="G52" s="7" t="n">
-        <v>8.68</v>
+        <v>3.79</v>
       </c>
       <c r="H52" s="8" t="inlineStr">
         <is>
-          <t>D26</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I52" s="9" t="inlineStr">
@@ -2269,11 +2269,11 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>45950.65608796296</v>
+        <v>45952.66378472222</v>
       </c>
       <c r="B53" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6502.82897</t>
+          <t>M.15608.6504.107621</t>
         </is>
       </c>
       <c r="C53" s="3" t="inlineStr">
@@ -2292,10 +2292,10 @@
         </is>
       </c>
       <c r="F53" s="6" t="n">
-        <v>97.85</v>
+        <v>39.46</v>
       </c>
       <c r="G53" s="7" t="n">
-        <v>9.79</v>
+        <v>3.95</v>
       </c>
       <c r="H53" s="8" t="inlineStr">
         <is>
@@ -2310,11 +2310,11 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>45950.64420138889</v>
+        <v>45952.63895833334</v>
       </c>
       <c r="B54" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6502.77625</t>
+          <t>M.15608.6504.78271</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr">
@@ -2333,14 +2333,14 @@
         </is>
       </c>
       <c r="F54" s="6" t="n">
-        <v>110.48</v>
+        <v>34.73</v>
       </c>
       <c r="G54" s="7" t="n">
-        <v>11.05</v>
+        <v>3.47</v>
       </c>
       <c r="H54" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>D26</t>
         </is>
       </c>
       <c r="I54" s="9" t="inlineStr">
@@ -2351,11 +2351,11 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>45950.5840625</v>
+        <v>45952.633784722224</v>
       </c>
       <c r="B55" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6502.40933</t>
+          <t>M.15608.6504.73385</t>
         </is>
       </c>
       <c r="C55" s="3" t="inlineStr">
@@ -2374,14 +2374,14 @@
         </is>
       </c>
       <c r="F55" s="6" t="n">
-        <v>14.2</v>
+        <v>14.21</v>
       </c>
       <c r="G55" s="7" t="n">
         <v>1.42</v>
       </c>
       <c r="H55" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>D33</t>
         </is>
       </c>
       <c r="I55" s="9" t="inlineStr">
@@ -2392,11 +2392,11 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>45950.56178240741</v>
+        <v>45952.586226851854</v>
       </c>
       <c r="B56" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6502.29309</t>
+          <t>M.15608.6504.45896</t>
         </is>
       </c>
       <c r="C56" s="3" t="inlineStr">
@@ -2415,14 +2415,14 @@
         </is>
       </c>
       <c r="F56" s="6" t="n">
-        <v>14.2</v>
+        <v>13.4</v>
       </c>
       <c r="G56" s="7" t="n">
-        <v>1.42</v>
+        <v>1.34</v>
       </c>
       <c r="H56" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I56" s="9" t="inlineStr">
@@ -2433,11 +2433,11 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>45950.46554398148</v>
+        <v>45952.560069444444</v>
       </c>
       <c r="B57" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6501.1419787</t>
+          <t>M.15608.6504.34027</t>
         </is>
       </c>
       <c r="C57" s="3" t="inlineStr">
@@ -2456,10 +2456,10 @@
         </is>
       </c>
       <c r="F57" s="6" t="n">
-        <v>29.99</v>
+        <v>36.3</v>
       </c>
       <c r="G57" s="7" t="n">
-        <v>3.0</v>
+        <v>3.63</v>
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
@@ -2474,11 +2474,11 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>45950.46275462963</v>
+        <v>45952.487858796296</v>
       </c>
       <c r="B58" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6501.1419548</t>
+          <t>M.15608.6503.1430691</t>
         </is>
       </c>
       <c r="C58" s="3" t="inlineStr">
@@ -2497,14 +2497,14 @@
         </is>
       </c>
       <c r="F58" s="6" t="n">
-        <v>31.57</v>
+        <v>104.35</v>
       </c>
       <c r="G58" s="7" t="n">
-        <v>3.16</v>
+        <v>10.44</v>
       </c>
       <c r="H58" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I58" s="9" t="inlineStr">
@@ -2515,11 +2515,11 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>45950.4056712963</v>
+        <v>45952.43483796297</v>
       </c>
       <c r="B59" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6501.1332454</t>
+          <t>M.15608.6503.1354508</t>
         </is>
       </c>
       <c r="C59" s="3" t="inlineStr">
@@ -2529,7 +2529,7 @@
       </c>
       <c r="D59" s="4" t="inlineStr">
         <is>
-          <t>Sale (Android App)</t>
+          <t>Sale (iOS App)</t>
         </is>
       </c>
       <c r="E59" s="5" t="inlineStr">
@@ -2538,14 +2538,14 @@
         </is>
       </c>
       <c r="F59" s="6" t="n">
-        <v>216.12</v>
+        <v>44.2</v>
       </c>
       <c r="G59" s="7" t="n">
-        <v>21.61</v>
+        <v>4.42</v>
       </c>
       <c r="H59" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I59" s="9" t="inlineStr">
@@ -2556,11 +2556,11 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>45950.19702546296</v>
+        <v>45952.12751157407</v>
       </c>
       <c r="B60" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6501.1064452</t>
+          <t>M.15608.6503.747194</t>
         </is>
       </c>
       <c r="C60" s="3" t="inlineStr">
@@ -2579,14 +2579,14 @@
         </is>
       </c>
       <c r="F60" s="6" t="n">
-        <v>146.08</v>
+        <v>45.78</v>
       </c>
       <c r="G60" s="7" t="n">
-        <v>14.61</v>
+        <v>4.58</v>
       </c>
       <c r="H60" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I60" s="9" t="inlineStr">
@@ -2597,11 +2597,11 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>45950.157222222224</v>
+        <v>45952.00640046296</v>
       </c>
       <c r="B61" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6501.994781</t>
+          <t>M.15608.6503.566392</t>
         </is>
       </c>
       <c r="C61" s="3" t="inlineStr">
@@ -2620,10 +2620,10 @@
         </is>
       </c>
       <c r="F61" s="6" t="n">
-        <v>26.83</v>
+        <v>43.22</v>
       </c>
       <c r="G61" s="7" t="n">
-        <v>2.68</v>
+        <v>4.32</v>
       </c>
       <c r="H61" s="8" t="inlineStr">
         <is>
@@ -2638,11 +2638,11 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>45950.07685185185</v>
+        <v>45951.95179398148</v>
       </c>
       <c r="B62" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6501.814016</t>
+          <t>M.15608.6503.460669</t>
         </is>
       </c>
       <c r="C62" s="3" t="inlineStr">
@@ -2661,14 +2661,14 @@
         </is>
       </c>
       <c r="F62" s="6" t="n">
-        <v>12.63</v>
+        <v>31.25</v>
       </c>
       <c r="G62" s="7" t="n">
-        <v>1.26</v>
+        <v>3.13</v>
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>D26</t>
         </is>
       </c>
       <c r="I62" s="9" t="inlineStr">
@@ -2679,11 +2679,11 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>45949.8775</v>
+        <v>45951.918599537035</v>
       </c>
       <c r="B63" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6501.327998</t>
+          <t>M.15608.6503.413344</t>
         </is>
       </c>
       <c r="C63" s="3" t="inlineStr">
@@ -2702,14 +2702,14 @@
         </is>
       </c>
       <c r="F63" s="6" t="n">
-        <v>146.08</v>
+        <v>26.83</v>
       </c>
       <c r="G63" s="7" t="n">
-        <v>14.61</v>
+        <v>2.68</v>
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>D26</t>
         </is>
       </c>
       <c r="I63" s="9" t="inlineStr">
@@ -2720,11 +2720,11 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>45949.66372685185</v>
+        <v>45951.695868055554</v>
       </c>
       <c r="B64" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6501.81033</t>
+          <t>M.15608.6503.127414</t>
         </is>
       </c>
       <c r="C64" s="3" t="inlineStr">
@@ -2734,7 +2734,7 @@
       </c>
       <c r="D64" s="4" t="inlineStr">
         <is>
-          <t>Sale (Android App)</t>
+          <t>Sale (iOS App)</t>
         </is>
       </c>
       <c r="E64" s="5" t="inlineStr">
@@ -2743,14 +2743,14 @@
         </is>
       </c>
       <c r="F64" s="6" t="n">
-        <v>50.86</v>
+        <v>14.21</v>
       </c>
       <c r="G64" s="7" t="n">
-        <v>5.09</v>
+        <v>1.42</v>
       </c>
       <c r="H64" s="8" t="inlineStr">
         <is>
-          <t>D26</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I64" s="9" t="inlineStr">
@@ -2761,11 +2761,11 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>45949.6209375</v>
+        <v>45951.63533564815</v>
       </c>
       <c r="B65" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6501.56619</t>
+          <t>M.15608.6503.85823</t>
         </is>
       </c>
       <c r="C65" s="3" t="inlineStr">
@@ -2784,14 +2784,14 @@
         </is>
       </c>
       <c r="F65" s="6" t="n">
-        <v>14.2</v>
+        <v>37.25</v>
       </c>
       <c r="G65" s="7" t="n">
-        <v>1.42</v>
+        <v>3.73</v>
       </c>
       <c r="H65" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I65" s="9" t="inlineStr">
@@ -2802,11 +2802,11 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>45949.43665509259</v>
+        <v>45951.47851851852</v>
       </c>
       <c r="B66" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6500.1219037</t>
+          <t>M.15608.6502.1404826</t>
         </is>
       </c>
       <c r="C66" s="3" t="inlineStr">
@@ -2825,14 +2825,14 @@
         </is>
       </c>
       <c r="F66" s="6" t="n">
-        <v>110.48</v>
+        <v>14.21</v>
       </c>
       <c r="G66" s="7" t="n">
-        <v>11.05</v>
+        <v>1.42</v>
       </c>
       <c r="H66" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>D33</t>
         </is>
       </c>
       <c r="I66" s="9" t="inlineStr">
@@ -2843,11 +2843,11 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>45949.43662037037</v>
+        <v>45951.430138888885</v>
       </c>
       <c r="B67" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6500.1219060</t>
+          <t>M.15608.6502.1343453</t>
         </is>
       </c>
       <c r="C67" s="3" t="inlineStr">
@@ -2857,7 +2857,7 @@
       </c>
       <c r="D67" s="4" t="inlineStr">
         <is>
-          <t>Sale (Android App)</t>
+          <t>Sale (iOS App)</t>
         </is>
       </c>
       <c r="E67" s="5" t="inlineStr">
@@ -2866,14 +2866,14 @@
         </is>
       </c>
       <c r="F67" s="6" t="n">
-        <v>14.2</v>
+        <v>36.3</v>
       </c>
       <c r="G67" s="7" t="n">
-        <v>1.42</v>
+        <v>3.63</v>
       </c>
       <c r="H67" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>D7</t>
         </is>
       </c>
       <c r="I67" s="9" t="inlineStr">
@@ -2884,11 +2884,11 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>45949.25372685185</v>
+        <v>45951.35328703704</v>
       </c>
       <c r="B68" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6500.1036240</t>
+          <t>M.15608.6502.1251979</t>
         </is>
       </c>
       <c r="C68" s="3" t="inlineStr">
@@ -2907,14 +2907,14 @@
         </is>
       </c>
       <c r="F68" s="6" t="n">
-        <v>29.99</v>
+        <v>110.49</v>
       </c>
       <c r="G68" s="7" t="n">
-        <v>3.0</v>
+        <v>11.05</v>
       </c>
       <c r="H68" s="8" t="inlineStr">
         <is>
-          <t>D24</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I68" s="9" t="inlineStr">
@@ -2924,43 +2924,84 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="B69" s="12" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C69" s="13" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D69" s="14" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E69" s="15" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="F69" s="16" t="n">
-        <v>3822.55</v>
-      </c>
-      <c r="G69" s="17" t="n">
-        <v>382.28</v>
-      </c>
-      <c r="H69" s="18" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="I69" s="19" t="inlineStr">
+      <c r="A69" s="1" t="n">
+        <v>45951.28636574074</v>
+      </c>
+      <c r="B69" s="2" t="inlineStr">
+        <is>
+          <t>M.15608.6502.1182640</t>
+        </is>
+      </c>
+      <c r="C69" s="3" t="inlineStr">
+        <is>
+          <t>Airalo - The World's First eSIM Store</t>
+        </is>
+      </c>
+      <c r="D69" s="4" t="inlineStr">
+        <is>
+          <t>Sale (iOS App)</t>
+        </is>
+      </c>
+      <c r="E69" s="5" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="F69" s="6" t="n">
+        <v>64.72</v>
+      </c>
+      <c r="G69" s="7" t="n">
+        <v>6.47</v>
+      </c>
+      <c r="H69" s="8" t="inlineStr">
+        <is>
+          <t>SAHS</t>
+        </is>
+      </c>
+      <c r="I69" s="9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B70" s="12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C70" s="13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D70" s="14" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E70" s="15" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F70" s="16" t="n">
+        <v>3622.88</v>
+      </c>
+      <c r="G70" s="17" t="n">
+        <v>362.31</v>
+      </c>
+      <c r="H70" s="18" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I70" s="19" t="inlineStr">
         <is>
           <t/>
         </is>

</xml_diff>